<commit_message>
added logging funcionality to the project
</commit_message>
<xml_diff>
--- a/glids.xlsx
+++ b/glids.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -836,6 +836,36 @@
         <v>45136.35345267361</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>bf4d</t>
+        </is>
+      </c>
+      <c r="D56" s="7" t="n">
+        <v>45136.36827644676</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>3151</t>
+        </is>
+      </c>
+      <c r="D57" s="7" t="n">
+        <v>45136.36828064814</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>f699</t>
+        </is>
+      </c>
+      <c r="D58" s="7" t="n">
+        <v>45136.36829612269</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>